<commit_message>
Refactor ExcelService and FileService to enhance Excel file processing capabilities, including flexible column configurations, improved error handling, and integration with FileService for file operations; update logging and validation methods.
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/data.xlsx
+++ b/src/main/resources/xlsx/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khai1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniAcad\src\main\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D55A67A-FDEA-43B8-96A3-9C7217495918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDFBAD9-7F9C-4928-A4FE-33CC4FA42A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>khai1234sd@gmail.com</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Đồng Tháp</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Huỳnh Phúc Thọ</t>
+  </si>
+  <si>
+    <t>Hậu Giang</t>
   </si>
 </sst>
 </file>
@@ -95,10 +104,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -115,6 +125,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1798319</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>860107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05EE5425-5A91-266A-F7B5-A9B57348FFD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6469380" y="426720"/>
+          <a:ext cx="1188719" cy="631507"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -318,19 +383,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="94.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -340,8 +406,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="3">
+        <v>38326</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -351,8 +420,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="3">
+        <v>37624</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -361,13 +433,32 @@
       </c>
       <c r="C4" t="s">
         <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>37226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>38292</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{8FEE95A1-7E2C-4216-8C71-BEBB9DCF4772}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{91F8054F-6569-4E7C-A474-9B7021C79A2E}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{79F8012D-26E2-4BF1-8BF2-1BF34F0DB3EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>